<commit_message>
update 12/7/2017 - relay from 10 to 6 - remote shutdown/startup - remove battery capacity & battery cycle life time - add seeder function from excel/csv - data updated remove irect1-16 - alarm log (alarm start/clear -> alarm active/deactive ) -
</commit_message>
<xml_diff>
--- a/public/DataLogTemplate.xlsx
+++ b/public/DataLogTemplate.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\lv_goldpower\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="20490" windowHeight="7515" xr2:uid="{BFA6D60B-EC70-4632-A870-ED769C5BA219}"/>
+    <workbookView xWindow="0" yWindow="3600" windowWidth="20490" windowHeight="7515"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>DATALOG  MONITORING</t>
   </si>
@@ -45,24 +45,6 @@
     <t>DATE /TIME</t>
   </si>
   <si>
-    <t>AC VOLTAGE</t>
-  </si>
-  <si>
-    <t>BUS VOLTAGE</t>
-  </si>
-  <si>
-    <t>RECTIFIER CURRENT</t>
-  </si>
-  <si>
-    <t>LOAD CURRENT</t>
-  </si>
-  <si>
-    <t>BATTERY CURRENT</t>
-  </si>
-  <si>
-    <t>BATTERY TEMP</t>
-  </si>
-  <si>
     <t>SITE ID</t>
   </si>
   <si>
@@ -72,14 +54,59 @@
     <t>ADDRESS</t>
   </si>
   <si>
-    <t>TOTAL RECTIFIER CURRENT</t>
+    <t>AC VOLTAGE (V)</t>
+  </si>
+  <si>
+    <t>BUS VOLTAGE (V)</t>
+  </si>
+  <si>
+    <r>
+      <t>BATTERY TEMP (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>°</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C)</t>
+    </r>
+  </si>
+  <si>
+    <t>BATTERY CURRENT (A)</t>
+  </si>
+  <si>
+    <t>LOAD CURRENT (A)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RECTIFIER CURRENT (A)</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>T</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +127,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -122,7 +155,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -131,46 +164,116 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -486,199 +589,156 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C1A036-B789-43DF-8863-416D17DC6563}">
-  <dimension ref="A1:X11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="X16" sqref="X16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
-    <col min="3" max="7" width="20.28515625" customWidth="1"/>
-    <col min="8" max="23" width="8.5703125" customWidth="1"/>
-    <col min="24" max="24" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="19.5703125" customWidth="1"/>
+    <col min="5" max="9" width="20.28515625" customWidth="1"/>
+    <col min="10" max="10" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="5" t="s">
+      <c r="C10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5"/>
-      <c r="W10" s="5"/>
-      <c r="X10" s="7" t="s">
+      <c r="H10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="2">
-        <v>1</v>
-      </c>
-      <c r="I11" s="2">
-        <v>2</v>
-      </c>
-      <c r="J11" s="2">
-        <v>3</v>
-      </c>
-      <c r="K11" s="2">
-        <v>4</v>
-      </c>
-      <c r="L11" s="2">
-        <v>5</v>
-      </c>
-      <c r="M11" s="2">
-        <v>6</v>
-      </c>
-      <c r="N11" s="2">
-        <v>7</v>
-      </c>
-      <c r="O11" s="2">
-        <v>8</v>
-      </c>
-      <c r="P11" s="2">
-        <v>9</v>
-      </c>
-      <c r="Q11" s="2">
-        <v>10</v>
-      </c>
-      <c r="R11" s="2">
-        <v>11</v>
-      </c>
-      <c r="S11" s="2">
-        <v>12</v>
-      </c>
-      <c r="T11" s="2">
-        <v>13</v>
-      </c>
-      <c r="U11" s="2">
-        <v>14</v>
-      </c>
-      <c r="V11" s="2">
-        <v>15</v>
-      </c>
-      <c r="W11" s="2">
+      <c r="D11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="X11" s="7"/>
+      <c r="E11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="X10:X11"/>
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="H10:W10"/>
+  <mergeCells count="9">
+    <mergeCell ref="J10:J11"/>
     <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="I10:I11"/>
     <mergeCell ref="A10:A11"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="A1:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>